<commit_message>
from stock to counter e.g:fstc
</commit_message>
<xml_diff>
--- a/Hira-Palace.xlsx
+++ b/Hira-Palace.xlsx
@@ -700,6 +700,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="6" applyFill="1"/>
     <xf numFmtId="44" fontId="5" fillId="24" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -749,9 +752,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -1078,28 +1078,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52" t="s">
+      <c r="E1" s="54"/>
+      <c r="F1" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52" t="s">
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="41" t="s">
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="42"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
@@ -1140,21 +1140,21 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -1478,21 +1478,21 @@
       <c r="M24" s="20"/>
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="45"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="48"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
@@ -1530,21 +1530,21 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="40"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
@@ -1591,21 +1591,21 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="40"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="s">
@@ -1643,21 +1643,21 @@
       </c>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="38"/>
-      <c r="K44" s="38"/>
-      <c r="L44" s="38"/>
-      <c r="M44" s="38"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
+      <c r="K44" s="41"/>
+      <c r="L44" s="41"/>
+      <c r="M44" s="41"/>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="s">
@@ -1668,21 +1668,21 @@
       </c>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="42"/>
+      <c r="L46" s="42"/>
+      <c r="M46" s="42"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
@@ -1811,28 +1811,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52" t="s">
+      <c r="E1" s="54"/>
+      <c r="F1" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52" t="s">
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="41" t="s">
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="42"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
@@ -1873,21 +1873,21 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -2211,21 +2211,21 @@
       <c r="M24" s="20"/>
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="45"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="48"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
@@ -2263,21 +2263,21 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="40"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
@@ -2324,21 +2324,21 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="40"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="s">
@@ -2376,21 +2376,21 @@
       </c>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="38"/>
-      <c r="K44" s="38"/>
-      <c r="L44" s="38"/>
-      <c r="M44" s="38"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
+      <c r="K44" s="41"/>
+      <c r="L44" s="41"/>
+      <c r="M44" s="41"/>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="s">
@@ -2401,21 +2401,21 @@
       </c>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="42"/>
+      <c r="L46" s="42"/>
+      <c r="M46" s="42"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
@@ -2508,17 +2508,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A25:M25"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A44:M44"/>
-    <mergeCell ref="A46:M46"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A44:M44"/>
+    <mergeCell ref="A46:M46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2530,7 +2530,7 @@
   <dimension ref="A1:Q55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2541,28 +2541,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52" t="s">
+      <c r="E1" s="54"/>
+      <c r="F1" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52" t="s">
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="41" t="s">
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="42"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
@@ -2603,21 +2603,21 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="P4">
         <f>SUM(B4:B23)</f>
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -2653,8 +2653,8 @@
         <v>14</v>
       </c>
       <c r="B5" s="13">
-        <f>1+3</f>
-        <v>4</v>
+        <f>1+3-3</f>
+        <v>1</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="8"/>
@@ -2719,8 +2719,8 @@
         <v>1</v>
       </c>
       <c r="B9" s="13">
-        <f>1+8</f>
-        <v>9</v>
+        <f>1+8-2</f>
+        <v>7</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="8"/>
@@ -2778,12 +2778,12 @@
       <c r="E12" s="9"/>
       <c r="I12" s="22"/>
       <c r="L12" s="24"/>
-      <c r="O12" s="53" t="s">
+      <c r="O12" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="P12" s="55">
+      <c r="P12" s="38">
         <f>SUM(P4:P11)</f>
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2791,8 +2791,8 @@
         <v>6</v>
       </c>
       <c r="B13" s="13">
-        <f>5+5*12</f>
-        <v>65</v>
+        <f>5+5*12-3</f>
+        <v>62</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="8"/>
@@ -2842,7 +2842,7 @@
       <c r="E16" s="4"/>
       <c r="I16" s="22"/>
       <c r="L16" s="24"/>
-      <c r="O16" s="54"/>
+      <c r="O16" s="37"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
@@ -2942,21 +2942,21 @@
       <c r="L23" s="24"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="45"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="48"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
@@ -3008,21 +3008,21 @@
       <c r="L31" s="24"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="40"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
@@ -3070,21 +3070,21 @@
       <c r="L37" s="24"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="37"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="40"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
@@ -3126,21 +3126,21 @@
       </c>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="38" t="s">
+      <c r="A43" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="41"/>
+      <c r="L43" s="41"/>
+      <c r="M43" s="41"/>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
@@ -3152,21 +3152,21 @@
       </c>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="42"/>
+      <c r="L45" s="42"/>
+      <c r="M45" s="42"/>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" t="s">
@@ -3277,17 +3277,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="A43:M43"/>
+    <mergeCell ref="A45:M45"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A32:M32"/>
-    <mergeCell ref="A38:M38"/>
-    <mergeCell ref="A43:M43"/>
-    <mergeCell ref="A45:M45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
missing one megic moment botol
</commit_message>
<xml_diff>
--- a/Hira-Palace.xlsx
+++ b/Hira-Palace.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="80">
   <si>
     <t>Black Dog</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>missing one bottol</t>
   </si>
 </sst>
 </file>
@@ -267,7 +270,7 @@
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$CHF-100C]_-;\-* #,##0.00\ [$CHF-100C]_-;_-* &quot;-&quot;??\ [$CHF-100C]_-;_-@_-"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +310,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -654,7 +664,7 @@
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -753,6 +763,8 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -3432,7 +3444,7 @@
       </c>
       <c r="P4">
         <f>SUM(B4:B23)</f>
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -3442,11 +3454,13 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="13">
-        <f>1+3-3-2</f>
-        <v>-1</v>
-      </c>
-      <c r="C5" s="11"/>
+      <c r="B5" s="57">
+        <f>1+3-3</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="I5" s="22"/>
@@ -3573,7 +3587,7 @@
       </c>
       <c r="P12" s="38">
         <f>SUM(P4:P11)</f>
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -3686,9 +3700,7 @@
       <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="13">
-        <v>-2</v>
-      </c>
+      <c r="B20" s="13"/>
       <c r="C20" s="11"/>
       <c r="D20" s="5"/>
       <c r="E20" s="4"/>
@@ -4089,5 +4101,6 @@
     <mergeCell ref="A3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
stock and counter update
</commit_message>
<xml_diff>
--- a/Hira-Palace.xlsx
+++ b/Hira-Palace.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="140" windowWidth="19140" windowHeight="7090"/>
+    <workbookView xWindow="80" yWindow="140" windowWidth="19140" windowHeight="7090" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="09-07-2023 (counter)" sheetId="7" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="08-07-2023" sheetId="2" r:id="rId4"/>
     <sheet name="09-07-2023" sheetId="5" r:id="rId5"/>
     <sheet name="09-07-2023 (stock)" sheetId="6" r:id="rId6"/>
+    <sheet name="10-07-2023 (stock)" sheetId="8" r:id="rId7"/>
+    <sheet name="10-07-2023 (counter)" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="90">
   <si>
     <t>Black Dog</t>
   </si>
@@ -777,6 +779,37 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -802,37 +835,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="24" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1146,7 +1148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -1167,32 +1169,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="57" t="s">
+      <c r="E1" s="57"/>
+      <c r="F1" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="62" t="s">
+      <c r="G1" s="53"/>
+      <c r="H1" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62" t="s">
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="63" t="s">
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="64"/>
+      <c r="O1" s="50"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
@@ -1249,23 +1251,23 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
       <c r="Q3" t="s">
         <v>81</v>
       </c>
@@ -1307,7 +1309,7 @@
       <c r="L4" s="22">
         <v>110</v>
       </c>
-      <c r="M4" s="67">
+      <c r="M4" s="48">
         <v>60</v>
       </c>
       <c r="N4" s="24">
@@ -2034,23 +2036,23 @@
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="51"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="62"/>
       <c r="P24">
         <f>SUM(C4:C23)</f>
         <v>2240</v>
@@ -2106,23 +2108,23 @@
       <c r="N31" s="24"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="52"/>
-      <c r="O32" s="52"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
@@ -2173,23 +2175,23 @@
       <c r="N37" s="24"/>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
-      <c r="M38" s="54"/>
-      <c r="N38" s="54"/>
-      <c r="O38" s="54"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
+      <c r="N38" s="65"/>
+      <c r="O38" s="65"/>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
@@ -2231,23 +2233,23 @@
       </c>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="55"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="55"/>
-      <c r="M43" s="55"/>
-      <c r="N43" s="55"/>
-      <c r="O43" s="55"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
+      <c r="N43" s="66"/>
+      <c r="O43" s="66"/>
     </row>
     <row r="44" spans="1:16">
       <c r="A44" t="s">
@@ -2259,23 +2261,23 @@
       </c>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="56" t="s">
+      <c r="A45" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
-      <c r="O45" s="56"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
+      <c r="M45" s="67"/>
+      <c r="N45" s="67"/>
+      <c r="O45" s="67"/>
     </row>
     <row r="46" spans="1:16">
       <c r="A46" t="s">
@@ -2408,6 +2410,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A32:O32"/>
+    <mergeCell ref="A38:O38"/>
+    <mergeCell ref="A43:O43"/>
+    <mergeCell ref="A45:O45"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="F1:G1"/>
@@ -2415,11 +2422,6 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
-    <mergeCell ref="A24:O24"/>
-    <mergeCell ref="A32:O32"/>
-    <mergeCell ref="A38:O38"/>
-    <mergeCell ref="A43:O43"/>
-    <mergeCell ref="A45:O45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2445,28 +2447,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62" t="s">
+      <c r="E1" s="57"/>
+      <c r="F1" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62" t="s">
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="63" t="s">
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="64"/>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
@@ -2507,21 +2509,21 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -2845,21 +2847,21 @@
       <c r="M24" s="20"/>
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="51"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="62"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
@@ -2897,21 +2899,21 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
@@ -2958,21 +2960,21 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="53" t="s">
+      <c r="A39" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="54"/>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="54"/>
-      <c r="M39" s="54"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="65"/>
+      <c r="J39" s="65"/>
+      <c r="K39" s="65"/>
+      <c r="L39" s="65"/>
+      <c r="M39" s="65"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="s">
@@ -3010,21 +3012,21 @@
       </c>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="55"/>
-      <c r="M44" s="55"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="66"/>
+      <c r="K44" s="66"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="66"/>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="s">
@@ -3035,21 +3037,21 @@
       </c>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="56" t="s">
+      <c r="A46" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="56"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="56"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="67"/>
+      <c r="J46" s="67"/>
+      <c r="K46" s="67"/>
+      <c r="L46" s="67"/>
+      <c r="M46" s="67"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
@@ -3178,28 +3180,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62" t="s">
+      <c r="E1" s="57"/>
+      <c r="F1" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62" t="s">
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="63" t="s">
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="64"/>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
@@ -3240,21 +3242,21 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -3578,21 +3580,21 @@
       <c r="M24" s="20"/>
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="51"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="62"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
@@ -3630,21 +3632,21 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
@@ -3691,21 +3693,21 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="53" t="s">
+      <c r="A39" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="54"/>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="54"/>
-      <c r="M39" s="54"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="65"/>
+      <c r="J39" s="65"/>
+      <c r="K39" s="65"/>
+      <c r="L39" s="65"/>
+      <c r="M39" s="65"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" t="s">
@@ -3743,21 +3745,21 @@
       </c>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="55"/>
-      <c r="M44" s="55"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="66"/>
+      <c r="K44" s="66"/>
+      <c r="L44" s="66"/>
+      <c r="M44" s="66"/>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" t="s">
@@ -3768,21 +3770,21 @@
       </c>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="56" t="s">
+      <c r="A46" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="56"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="56"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="67"/>
+      <c r="J46" s="67"/>
+      <c r="K46" s="67"/>
+      <c r="L46" s="67"/>
+      <c r="M46" s="67"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" t="s">
@@ -3875,17 +3877,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A44:M44"/>
+    <mergeCell ref="A46:M46"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="A25:M25"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="A44:M44"/>
-    <mergeCell ref="A46:M46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3910,28 +3912,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62" t="s">
+      <c r="E1" s="57"/>
+      <c r="F1" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62" t="s">
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="63" t="s">
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="64"/>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
@@ -3972,21 +3974,21 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -4311,21 +4313,21 @@
       <c r="L23" s="24"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="51"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="62"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
@@ -4377,21 +4379,21 @@
       <c r="L31" s="24"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
@@ -4446,21 +4448,21 @@
       <c r="L37" s="24"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
-      <c r="M38" s="54"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
@@ -4502,21 +4504,21 @@
       </c>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="55"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="55"/>
-      <c r="M43" s="55"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
@@ -4528,21 +4530,21 @@
       </c>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="56" t="s">
+      <c r="A45" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
+      <c r="M45" s="67"/>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" t="s">
@@ -4658,17 +4660,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A32:M32"/>
-    <mergeCell ref="A38:M38"/>
-    <mergeCell ref="A43:M43"/>
-    <mergeCell ref="A45:M45"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="A43:M43"/>
+    <mergeCell ref="A45:M45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4692,28 +4694,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62" t="s">
+      <c r="E1" s="57"/>
+      <c r="F1" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62" t="s">
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="63" t="s">
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="64"/>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
@@ -4754,21 +4756,21 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -5102,21 +5104,21 @@
       <c r="L23" s="24"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="51"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="62"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
@@ -5168,21 +5170,21 @@
       <c r="L31" s="24"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
@@ -5243,21 +5245,21 @@
       <c r="L37" s="24"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
-      <c r="M38" s="54"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
@@ -5299,21 +5301,21 @@
       </c>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="55"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="55"/>
-      <c r="M43" s="55"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" t="s">
@@ -5325,21 +5327,21 @@
       </c>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="56" t="s">
+      <c r="A45" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
+      <c r="M45" s="67"/>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" t="s">
@@ -5450,17 +5452,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A32:M32"/>
-    <mergeCell ref="A38:M38"/>
-    <mergeCell ref="A43:M43"/>
-    <mergeCell ref="A45:M45"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="A43:M43"/>
+    <mergeCell ref="A45:M45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5486,28 +5488,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62" t="s">
+      <c r="E1" s="57"/>
+      <c r="F1" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62" t="s">
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="63" t="s">
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="64"/>
+      <c r="M1" s="50"/>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
@@ -5555,21 +5557,21 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
       <c r="O3" t="s">
         <v>81</v>
       </c>
@@ -5924,21 +5926,21 @@
       <c r="L23" s="24"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="51"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="62"/>
       <c r="N24">
         <f>SUM(C4:C23)</f>
         <v>2240</v>
@@ -5994,21 +5996,21 @@
       <c r="L31" s="24"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
@@ -6069,21 +6071,21 @@
       <c r="L37" s="24"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
-      <c r="M38" s="54"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" t="s">
@@ -6125,21 +6127,21 @@
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="55"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="55"/>
-      <c r="M43" s="55"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
@@ -6151,21 +6153,21 @@
       </c>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="56" t="s">
+      <c r="A45" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
+      <c r="M45" s="67"/>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" t="s">
@@ -6281,17 +6283,2135 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="A43:M43"/>
+    <mergeCell ref="A45:M45"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.08984375" customWidth="1"/>
+    <col min="16" max="16" width="11.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="B1" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="57"/>
+      <c r="F1" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="50"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2">
+        <f>SUM(C4:C23)</f>
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="O3" t="s">
+        <v>81</v>
+      </c>
+      <c r="P3">
+        <f>SUM(B4:B23)</f>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="12">
+        <f>119-1-2</f>
+        <v>116</v>
+      </c>
+      <c r="C4" s="11">
+        <v>500</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="I4" s="22">
+        <v>710</v>
+      </c>
+      <c r="L4" s="24">
+        <f>B4*I4</f>
+        <v>82360</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4">
+        <f>SUM(B4:B23)</f>
+        <v>183</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="41">
+        <v>1</v>
+      </c>
+      <c r="C5" s="42">
+        <v>900</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="I5" s="22">
+        <v>880</v>
+      </c>
+      <c r="L5" s="24">
+        <f>B5*I5</f>
+        <v>880</v>
+      </c>
+      <c r="O5" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="L6" s="24"/>
+      <c r="O6" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6">
+        <f>SUM(B46:B55)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="I7" s="22">
+        <v>1900</v>
+      </c>
+      <c r="L7" s="24">
+        <f>B7*I7</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="11">
+        <v>600</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="I8" s="22"/>
+      <c r="L8" s="24"/>
+      <c r="O8" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13">
+        <v>9</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="I9" s="22">
+        <v>880</v>
+      </c>
+      <c r="L9" s="24">
+        <f>B9*I9</f>
+        <v>7920</v>
+      </c>
+      <c r="M9" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="I10" s="22">
+        <v>880</v>
+      </c>
+      <c r="L10" s="24">
+        <f>B10*I10</f>
+        <v>880</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="13">
+        <v>4</v>
+      </c>
+      <c r="C11" s="11">
+        <v>180</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="I11" s="22"/>
+      <c r="L11" s="24"/>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11">
+        <v>60</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="L12" s="24"/>
+      <c r="O12" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="P12" s="38">
+        <f>SUM(P4:P11)</f>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="13">
+        <f>52-2</f>
+        <v>50</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="I13" s="22">
+        <v>880</v>
+      </c>
+      <c r="L13" s="24">
+        <f>B13*I13</f>
+        <v>44000</v>
+      </c>
+      <c r="M13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="I14" s="22"/>
+      <c r="L14" s="24"/>
+      <c r="M14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4"/>
+      <c r="I15" s="22"/>
+      <c r="L15" s="24"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="I16" s="22"/>
+      <c r="L16" s="24"/>
+      <c r="O16" s="37"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="I17" s="22"/>
+      <c r="L17" s="24"/>
+      <c r="M17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="I18" s="22"/>
+      <c r="L18" s="24"/>
+      <c r="M18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4"/>
+      <c r="I19" s="22"/>
+      <c r="L19" s="24"/>
+      <c r="M19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="4"/>
+      <c r="I20" s="22"/>
+      <c r="L20" s="24"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="I21" s="22"/>
+      <c r="L21" s="24"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="I22" s="22"/>
+      <c r="L22" s="24"/>
+      <c r="M22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="I23" s="22"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="62"/>
+      <c r="N24">
+        <f>SUM(C4:C23)</f>
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="22"/>
+      <c r="L25" s="24"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" s="22"/>
+      <c r="L26" s="24"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="22"/>
+      <c r="L27" s="24"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" s="22"/>
+      <c r="L28" s="24"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29" s="22"/>
+      <c r="L29" s="24"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="22"/>
+      <c r="L30" s="24"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="22"/>
+      <c r="L31" s="24"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33">
+        <v>57</v>
+      </c>
+      <c r="F33" s="24">
+        <v>400</v>
+      </c>
+      <c r="I33" s="24">
+        <v>230</v>
+      </c>
+      <c r="L33" s="24">
+        <f>I33*B33</f>
+        <v>13110</v>
+      </c>
+      <c r="M33" s="22">
+        <f>F33*B33</f>
+        <v>22800</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="I34" s="22">
+        <v>320</v>
+      </c>
+      <c r="L34" s="24"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="I35" s="22">
+        <v>320</v>
+      </c>
+      <c r="L35" s="24"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="I36" s="22">
+        <v>400</v>
+      </c>
+      <c r="L36" s="24"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="I37" s="22">
+        <v>320</v>
+      </c>
+      <c r="L37" s="24"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+      <c r="I39" s="22"/>
+      <c r="L39" s="22">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="22"/>
+      <c r="L40" s="22">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
+      <c r="I41" s="22"/>
+      <c r="L41" s="22">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="I42" s="22"/>
+      <c r="L42" s="22">
+        <v>190</v>
+      </c>
+      <c r="M42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="I44" s="22"/>
+      <c r="L44" s="24">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="67"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
+      <c r="M45" s="67"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46">
+        <v>300</v>
+      </c>
+      <c r="I46" s="22"/>
+      <c r="L46" s="24">
+        <v>350</v>
+      </c>
+      <c r="N46">
+        <f>SUM(C4:C23)+SUM(C46:C54)</f>
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" t="s">
+        <v>71</v>
+      </c>
+      <c r="I47" s="22"/>
+      <c r="L47" s="24">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="13">
+        <v>1</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="I48" s="22"/>
+      <c r="L48" s="24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" t="s">
+        <v>72</v>
+      </c>
+      <c r="I49" s="22"/>
+      <c r="L49" s="24">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="13">
+        <v>700</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="9"/>
+      <c r="I50" s="22"/>
+      <c r="L50" s="24">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="4"/>
+      <c r="I51" s="22"/>
+      <c r="L51" s="24">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="I52" s="22"/>
+      <c r="L52" s="24"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="4"/>
+      <c r="I53" s="22"/>
+      <c r="L53" s="24"/>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="10"/>
+      <c r="C54" s="11">
+        <v>600</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="6"/>
+      <c r="I54" s="22"/>
+      <c r="L54" s="24"/>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
     <mergeCell ref="A24:M24"/>
     <mergeCell ref="A32:M32"/>
     <mergeCell ref="A38:M38"/>
     <mergeCell ref="A43:M43"/>
     <mergeCell ref="A45:M45"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="18.90625" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" customWidth="1"/>
+    <col min="15" max="15" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.08984375" customWidth="1"/>
+    <col min="18" max="18" width="11.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="B1" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="57"/>
+      <c r="F1" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="53"/>
+      <c r="H1" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="50"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2">
+        <f>SUM(C4:C23)</f>
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="Q3" t="s">
+        <v>81</v>
+      </c>
+      <c r="R3">
+        <f>SUM(B4:B23)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="12">
+        <f>4+2</f>
+        <v>6</v>
+      </c>
+      <c r="C4" s="11">
+        <v>500</v>
+      </c>
+      <c r="D4" s="46">
+        <f>IF(C4&gt;60,B4+1,B4)</f>
+        <v>7</v>
+      </c>
+      <c r="E4" s="46">
+        <f>750*B4+C4</f>
+        <v>5000</v>
+      </c>
+      <c r="F4" s="46">
+        <f>ROUND((750*B4+C4)/60,0)</f>
+        <v>83</v>
+      </c>
+      <c r="G4" s="46">
+        <f>750/60</f>
+        <v>12.5</v>
+      </c>
+      <c r="K4" s="22">
+        <f>G4*L4</f>
+        <v>1375</v>
+      </c>
+      <c r="L4" s="22">
+        <v>110</v>
+      </c>
+      <c r="M4" s="48">
+        <v>60</v>
+      </c>
+      <c r="N4" s="24">
+        <f>F4*L4</f>
+        <v>9130</v>
+      </c>
+      <c r="O4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="R4">
+        <f>SUM(B4:B23)</f>
+        <v>25</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="41">
+        <v>1</v>
+      </c>
+      <c r="C5" s="42">
+        <v>900</v>
+      </c>
+      <c r="D5" s="46">
+        <f t="shared" ref="D5:D23" si="0">IF(C5&gt;60,B5+1,B5)</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="46">
+        <f t="shared" ref="E5:E23" si="1">750*B5+C5</f>
+        <v>1650</v>
+      </c>
+      <c r="F5" s="46">
+        <f t="shared" ref="F5:F23" si="2">ROUND((750*B5+C5)/60,0)</f>
+        <v>28</v>
+      </c>
+      <c r="G5" s="46">
+        <f t="shared" ref="G5:G23" si="3">750/60</f>
+        <v>12.5</v>
+      </c>
+      <c r="K5" s="22">
+        <f t="shared" ref="K5:K22" si="4">G5*L5</f>
+        <v>2500</v>
+      </c>
+      <c r="L5" s="22">
+        <v>200</v>
+      </c>
+      <c r="N5" s="24">
+        <f t="shared" ref="N5:N23" si="5">F5*L5</f>
+        <v>5600</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K6" s="22">
+        <f t="shared" si="4"/>
+        <v>4375</v>
+      </c>
+      <c r="L6" s="22">
+        <v>350</v>
+      </c>
+      <c r="N6" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6">
+        <f>SUM(B46:B55)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K7" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="11">
+        <v>600</v>
+      </c>
+      <c r="D8" s="46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="46">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="F8" s="46">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G8" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K8" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13">
+        <v>3</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="46">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E9" s="46">
+        <f t="shared" si="1"/>
+        <v>2250</v>
+      </c>
+      <c r="F9" s="46">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="G9" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K9" s="22">
+        <f t="shared" si="4"/>
+        <v>1625</v>
+      </c>
+      <c r="L9" s="22">
+        <v>130</v>
+      </c>
+      <c r="N9" s="24">
+        <f t="shared" si="5"/>
+        <v>4940</v>
+      </c>
+      <c r="O9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q9" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="46">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
+      <c r="F10" s="46">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="G10" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K10" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="13">
+        <v>4</v>
+      </c>
+      <c r="C11" s="11">
+        <v>180</v>
+      </c>
+      <c r="D11" s="46">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E11" s="46">
+        <f t="shared" si="1"/>
+        <v>3180</v>
+      </c>
+      <c r="F11" s="46">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="G11" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K11" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11">
+        <v>60</v>
+      </c>
+      <c r="D12" s="46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="46">
+        <f t="shared" si="1"/>
+        <v>810</v>
+      </c>
+      <c r="F12" s="46">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G12" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K12" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="R12" s="38">
+        <f>SUM(R4:R11)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="13">
+        <f>3+5</f>
+        <v>8</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="46">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E13" s="46">
+        <f t="shared" si="1"/>
+        <v>6000</v>
+      </c>
+      <c r="F13" s="46">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G13" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K13" s="22">
+        <f t="shared" si="4"/>
+        <v>1625</v>
+      </c>
+      <c r="L13" s="22">
+        <v>130</v>
+      </c>
+      <c r="N13" s="24">
+        <f t="shared" si="5"/>
+        <v>13000</v>
+      </c>
+      <c r="O13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="46">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
+      <c r="F14" s="46">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="G14" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K14" s="22">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="L14" s="22">
+        <v>160</v>
+      </c>
+      <c r="N14" s="24">
+        <f t="shared" si="5"/>
+        <v>2080</v>
+      </c>
+      <c r="O14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K15" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K16" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f>12.3*B4+C4/60</f>
+        <v>82.13333333333334</v>
+      </c>
+      <c r="R16" s="22">
+        <v>110</v>
+      </c>
+      <c r="S16" s="22">
+        <f>R16*Q16</f>
+        <v>9034.6666666666679</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K17" s="22">
+        <f t="shared" si="4"/>
+        <v>2500</v>
+      </c>
+      <c r="L17" s="22">
+        <v>200</v>
+      </c>
+      <c r="N17" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K18" s="22">
+        <f t="shared" si="4"/>
+        <v>2250</v>
+      </c>
+      <c r="L18" s="22">
+        <v>180</v>
+      </c>
+      <c r="N18" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K19" s="22">
+        <f t="shared" si="4"/>
+        <v>1875</v>
+      </c>
+      <c r="L19" s="22">
+        <v>150</v>
+      </c>
+      <c r="N19" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K20" s="22">
+        <f t="shared" si="4"/>
+        <v>2125</v>
+      </c>
+      <c r="L20" s="22">
+        <v>170</v>
+      </c>
+      <c r="N20" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K21" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K22" s="22">
+        <f t="shared" si="4"/>
+        <v>1375</v>
+      </c>
+      <c r="L22" s="22">
+        <v>110</v>
+      </c>
+      <c r="N22" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="46">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="K23" s="22"/>
+      <c r="N23" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="62"/>
+      <c r="P24">
+        <f>SUM(C4:C23)</f>
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="22"/>
+      <c r="N25" s="24"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" s="22"/>
+      <c r="N26" s="24"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="22"/>
+      <c r="N27" s="24"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" s="22"/>
+      <c r="N28" s="24"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="K29" s="22"/>
+      <c r="N29" s="24"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="K30" s="22"/>
+      <c r="N30" s="24"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="22"/>
+      <c r="N31" s="24"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33">
+        <v>57</v>
+      </c>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24">
+        <v>400</v>
+      </c>
+      <c r="N33" s="24" t="e">
+        <f>#REF!*B33</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O33" s="22">
+        <f>L33*B33</f>
+        <v>22800</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="K34" s="22"/>
+      <c r="N34" s="24"/>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="K35" s="22"/>
+      <c r="N35" s="24"/>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="K36" s="22"/>
+      <c r="N36" s="24"/>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="K37" s="22"/>
+      <c r="N37" s="24"/>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
+      <c r="N38" s="65"/>
+      <c r="O38" s="65"/>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22">
+        <v>190</v>
+      </c>
+      <c r="O42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="66"/>
+      <c r="M43" s="66"/>
+      <c r="N43" s="66"/>
+      <c r="O43" s="66"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="K44" s="22"/>
+      <c r="L44" s="24">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="67"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
+      <c r="M45" s="67"/>
+      <c r="N45" s="67"/>
+      <c r="O45" s="67"/>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46">
+        <v>300</v>
+      </c>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22">
+        <v>350</v>
+      </c>
+      <c r="N46" s="24"/>
+      <c r="P46">
+        <f>SUM(C4:C23)+SUM(C46:C54)</f>
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" t="s">
+        <v>71</v>
+      </c>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22">
+        <v>550</v>
+      </c>
+      <c r="N47" s="24"/>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="43">
+        <v>1</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22">
+        <v>1000</v>
+      </c>
+      <c r="N48" s="24"/>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="44"/>
+      <c r="K49" s="22"/>
+      <c r="L49" s="24">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="44"/>
+      <c r="C50" s="13">
+        <v>700</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="24">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="43"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="24">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="44"/>
+      <c r="K52" s="22"/>
+      <c r="N52" s="24"/>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="43"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="K53" s="22"/>
+      <c r="N53" s="24"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="45"/>
+      <c r="C54" s="11">
+        <v>600</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="K54" s="22"/>
+      <c r="N54" s="24"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A24:O24"/>
+    <mergeCell ref="A32:O32"/>
+    <mergeCell ref="A38:O38"/>
+    <mergeCell ref="A43:O43"/>
+    <mergeCell ref="A45:O45"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>